<commit_message>
Se simplifica el modelo desde el punto de vista de los agrupadores. Solo hay dos (taller y almuerzo del personal de servicio) y se elimina el tipo de agrupador. Era excesiva información y no aportaba valor.
</commit_message>
<xml_diff>
--- a/03 - Base de datos/excel/01 - Tablas de parámetros.xlsx
+++ b/03 - Base de datos/excel/01 - Tablas de parámetros.xlsx
@@ -1,28 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26327"/>
   <workbookPr showInkAnnotation="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrador\Dropbox\Desarrollo de software\DuocUC\PTY4478 - Portafolio\Base de datos\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrador\Documents\Software\Duoc\admtaller-bd\03 - Base de datos\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC6DC617-FA6E-4773-B011-B960188D3705}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A85FDB38-F30D-4A51-97AA-013F87B7DD06}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="3" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="tipo_agrupador" sheetId="1" r:id="rId1"/>
-    <sheet name="agrupador" sheetId="3" r:id="rId2"/>
-    <sheet name="periodo_academ" sheetId="11" r:id="rId3"/>
-    <sheet name="carrera" sheetId="4" r:id="rId4"/>
-    <sheet name="categ_producto" sheetId="5" r:id="rId5"/>
-    <sheet name="unidad_medida" sheetId="6" r:id="rId6"/>
-    <sheet name="asign" sheetId="7" r:id="rId7"/>
-    <sheet name="perfil" sheetId="8" r:id="rId8"/>
-    <sheet name="item_menu" sheetId="12" r:id="rId9"/>
-    <sheet name="config_perfil" sheetId="13" r:id="rId10"/>
+    <sheet name="agrupador" sheetId="3" r:id="rId1"/>
+    <sheet name="periodo_academ" sheetId="11" r:id="rId2"/>
+    <sheet name="carrera" sheetId="4" r:id="rId3"/>
+    <sheet name="categ_producto" sheetId="5" r:id="rId4"/>
+    <sheet name="unidad_medida" sheetId="6" r:id="rId5"/>
+    <sheet name="asign" sheetId="7" r:id="rId6"/>
+    <sheet name="perfil" sheetId="8" r:id="rId7"/>
+    <sheet name="item_menu" sheetId="12" r:id="rId8"/>
+    <sheet name="config_perfil" sheetId="13" r:id="rId9"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -34,16 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="362" uniqueCount="208">
-  <si>
-    <t>cod_tipo_agrupador</t>
-  </si>
-  <si>
-    <t>nom_tipo_agrupador</t>
-  </si>
-  <si>
-    <t>Almuerzo de servicio</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="341" uniqueCount="190">
   <si>
     <t>tabla</t>
   </si>
@@ -51,9 +41,6 @@
     <t>insert</t>
   </si>
   <si>
-    <t>tipo_agrupador</t>
-  </si>
-  <si>
     <t>agrupador</t>
   </si>
   <si>
@@ -63,45 +50,6 @@
     <t>nom_agrupador</t>
   </si>
   <si>
-    <t>Menú: Garbanzos con longaniza y postre</t>
-  </si>
-  <si>
-    <t>Menú: Pescado al horno y puré de papas y postre</t>
-  </si>
-  <si>
-    <t>Menú: Vacuno Bourguignon, papas asadas y postre</t>
-  </si>
-  <si>
-    <t>Menú: Pasta con salsa de champiñón, aceitunas, perejil y postre</t>
-  </si>
-  <si>
-    <t>Menú: Zapallo italiano relleno o guiso, arroz y postre</t>
-  </si>
-  <si>
-    <t>Menú: Pastel de papa y postre</t>
-  </si>
-  <si>
-    <t>Menú: charquicán y huevo frito, ensalada y postre</t>
-  </si>
-  <si>
-    <t>Menú: garbanzos con longaniza, ensalada y postre</t>
-  </si>
-  <si>
-    <t>Menú: lentejas con gorda, ensalada y postre</t>
-  </si>
-  <si>
-    <t>Menú: pescado horno, puré, ensalada y postre</t>
-  </si>
-  <si>
-    <t>Menú: pizza y postre</t>
-  </si>
-  <si>
-    <t>Menú: pollo arvejado y papas doradas, ensalada y postre</t>
-  </si>
-  <si>
-    <t>Menú: pollo asado con puré de papas, ensalada y postre</t>
-  </si>
-  <si>
     <t>carrera</t>
   </si>
   <si>
@@ -159,9 +107,6 @@
     <t>Vinos, licores y bebidas</t>
   </si>
   <si>
-    <t>Menú: Arroz chaufa de pollo y postre</t>
-  </si>
-  <si>
     <t>GASTRO</t>
   </si>
   <si>
@@ -435,12 +380,6 @@
     <t>TAV</t>
   </si>
   <si>
-    <t>(Sin tipo de agrupación)</t>
-  </si>
-  <si>
-    <t>(Sin agrupación)</t>
-  </si>
-  <si>
     <t>Administrador de carrera</t>
   </si>
   <si>
@@ -658,6 +597,12 @@
   </si>
   <si>
     <t>/productos/lista/</t>
+  </si>
+  <si>
+    <t>Almuerzo personal de servicio</t>
+  </si>
+  <si>
+    <t>Taller</t>
   </si>
 </sst>
 </file>
@@ -1008,134 +953,45 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{184DDF2A-1EF7-4716-8FBE-A79DA735D726}">
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3:C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="18.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="72.5703125" style="2" customWidth="1"/>
-    <col min="4" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" width="18.81640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="58.26953125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="72.54296875" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>0</v>
-      </c>
       <c r="B2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" ht="78.75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:3" ht="94.5" x14ac:dyDescent="0.35">
       <c r="A3" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="C3" s="2" t="str">
-        <f>"insert into "&amp;B1&amp;" ("&amp;CHAR(10)&amp;
-CHAR(9)&amp;$A2&amp;","&amp;CHAR(10)&amp;
-CHAR(9)&amp;$B2&amp;")"&amp;CHAR(10)&amp;
-"values ("&amp;CHAR(10)&amp;
-CHAR(9)&amp;A3&amp;","&amp;CHAR(10)&amp;
-CHAR(9)&amp;"'"&amp;B3&amp;"');"&amp;CHAR(10)</f>
-        <v xml:space="preserve">insert into tipo_agrupador (
-	cod_tipo_agrupador,
-	nom_tipo_agrupador)
-values (
-	0,
-	'(Sin tipo de agrupación)');
-</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" ht="78.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="1">
-        <v>1</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C4" s="2" t="str">
-        <f>"insert into "&amp;B2&amp;" ("&amp;CHAR(10)&amp;
-CHAR(9)&amp;$A3&amp;","&amp;CHAR(10)&amp;
-CHAR(9)&amp;$B3&amp;")"&amp;CHAR(10)&amp;
-"values ("&amp;CHAR(10)&amp;
-CHAR(9)&amp;A4&amp;","&amp;CHAR(10)&amp;
-CHAR(9)&amp;"'"&amp;B4&amp;"');"&amp;CHAR(10)</f>
-        <v xml:space="preserve">insert into nom_tipo_agrupador (
-	0,
-	(Sin tipo de agrupación))
-values (
-	1,
-	'Almuerzo de servicio');
-</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7280E62-DF8A-463C-91EE-0993A8577DEA}">
-  <dimension ref="A1:C46"/>
-  <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A41" workbookViewId="0">
-      <selection activeCell="A47" sqref="A47"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="18.85546875" style="6" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="26.85546875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="72.5703125" style="1" customWidth="1"/>
-    <col min="4" max="16384" width="11.42578125" style="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>181</v>
-      </c>
-      <c r="C1" s="2"/>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="5" t="s">
-        <v>114</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" ht="78.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="6" t="s">
-        <v>182</v>
-      </c>
-      <c r="B3" s="6" t="s">
-        <v>140</v>
+        <v>189</v>
       </c>
       <c r="C3" s="2" t="str">
         <f>"insert into "&amp;B$1&amp;" ("&amp;CHAR(10)&amp;
@@ -1144,1254 +1000,90 @@
 "values ("&amp;CHAR(10)&amp;
 CHAR(9)&amp;A3&amp;","&amp;CHAR(10)&amp;
 CHAR(9)&amp;"'"&amp;B3&amp;"');"&amp;CHAR(10)</f>
-        <v xml:space="preserve">insert into config_perfil (
-	cod_perfil,
-	cod_item_menu)
-values (
-	0,
-	'01');
-</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" ht="78.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="6" t="s">
-        <v>182</v>
-      </c>
-      <c r="B4" s="6" t="s">
-        <v>187</v>
+        <v xml:space="preserve">insert into agrupador (
+	cod_agrupador,
+	nom_agrupador)
+values (
+	1,
+	'Taller');
+</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="73.5" x14ac:dyDescent="0.35">
+      <c r="A4" s="1">
+        <v>2</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>188</v>
       </c>
       <c r="C4" s="2" t="str">
-        <f t="shared" ref="C4:C46" si="0">"insert into "&amp;B$1&amp;" ("&amp;CHAR(10)&amp;
+        <f>"insert into "&amp;B$1&amp;" ("&amp;CHAR(10)&amp;
 CHAR(9)&amp;$A$2&amp;","&amp;CHAR(10)&amp;
 CHAR(9)&amp;$B$2&amp;")"&amp;CHAR(10)&amp;
 "values ("&amp;CHAR(10)&amp;
 CHAR(9)&amp;A4&amp;","&amp;CHAR(10)&amp;
 CHAR(9)&amp;"'"&amp;B4&amp;"');"&amp;CHAR(10)</f>
-        <v xml:space="preserve">insert into config_perfil (
-	cod_perfil,
-	cod_item_menu)
-values (
-	0,
-	'0101');
-</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" ht="78.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="6" t="s">
-        <v>182</v>
-      </c>
-      <c r="B5" s="6" t="s">
-        <v>188</v>
-      </c>
-      <c r="C5" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">insert into config_perfil (
-	cod_perfil,
-	cod_item_menu)
-values (
-	0,
-	'0102');
-</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" ht="78.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="6" t="s">
-        <v>182</v>
-      </c>
-      <c r="B6" s="6" t="s">
-        <v>189</v>
-      </c>
-      <c r="C6" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">insert into config_perfil (
-	cod_perfil,
-	cod_item_menu)
-values (
-	0,
-	'0103');
-</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" ht="78.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="6" t="s">
-        <v>182</v>
-      </c>
-      <c r="B7" s="6" t="s">
-        <v>192</v>
-      </c>
-      <c r="C7" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">insert into config_perfil (
-	cod_perfil,
-	cod_item_menu)
-values (
-	0,
-	'0104');
-</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" ht="78.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="6" t="s">
-        <v>182</v>
-      </c>
-      <c r="B8" s="6" t="s">
-        <v>193</v>
-      </c>
-      <c r="C8" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">insert into config_perfil (
-	cod_perfil,
-	cod_item_menu)
-values (
-	0,
-	'0105');
-</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" ht="78.75" x14ac:dyDescent="0.25">
-      <c r="A9" s="6" t="s">
-        <v>182</v>
-      </c>
-      <c r="B9" s="6" t="s">
-        <v>194</v>
-      </c>
-      <c r="C9" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">insert into config_perfil (
-	cod_perfil,
-	cod_item_menu)
-values (
-	0,
-	'0106');
-</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" ht="78.75" x14ac:dyDescent="0.25">
-      <c r="A10" s="6" t="s">
-        <v>182</v>
-      </c>
-      <c r="B10" s="6" t="s">
-        <v>195</v>
-      </c>
-      <c r="C10" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">insert into config_perfil (
-	cod_perfil,
-	cod_item_menu)
-values (
-	0,
-	'0107');
-</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" ht="78.75" x14ac:dyDescent="0.25">
-      <c r="A11" s="6" t="s">
-        <v>182</v>
-      </c>
-      <c r="B11" s="6" t="s">
-        <v>206</v>
-      </c>
-      <c r="C11" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">insert into config_perfil (
-	cod_perfil,
-	cod_item_menu)
-values (
-	0,
-	'0108');
-</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" ht="78.75" x14ac:dyDescent="0.25">
-      <c r="A12" s="6" t="s">
-        <v>182</v>
-      </c>
-      <c r="B12" s="6" t="s">
-        <v>144</v>
-      </c>
-      <c r="C12" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">insert into config_perfil (
-	cod_perfil,
-	cod_item_menu)
-values (
-	0,
-	'02');
-</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" ht="78.75" x14ac:dyDescent="0.25">
-      <c r="A13" s="6" t="s">
-        <v>182</v>
-      </c>
-      <c r="B13" s="6" t="s">
-        <v>201</v>
-      </c>
-      <c r="C13" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">insert into config_perfil (
-	cod_perfil,
-	cod_item_menu)
-values (
-	0,
-	'0201');
-</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" ht="78.75" x14ac:dyDescent="0.25">
-      <c r="A14" s="6" t="s">
-        <v>182</v>
-      </c>
-      <c r="B14" s="6" t="s">
-        <v>202</v>
-      </c>
-      <c r="C14" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">insert into config_perfil (
-	cod_perfil,
-	cod_item_menu)
-values (
-	0,
-	'0202');
-</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" ht="78.75" x14ac:dyDescent="0.25">
-      <c r="A15" s="6" t="s">
-        <v>182</v>
-      </c>
-      <c r="B15" s="6" t="s">
-        <v>203</v>
-      </c>
-      <c r="C15" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">insert into config_perfil (
-	cod_perfil,
-	cod_item_menu)
-values (
-	0,
-	'0203');
-</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" ht="78.75" x14ac:dyDescent="0.25">
-      <c r="A16" s="6" t="s">
-        <v>182</v>
-      </c>
-      <c r="B16" s="6" t="s">
-        <v>204</v>
-      </c>
-      <c r="C16" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">insert into config_perfil (
-	cod_perfil,
-	cod_item_menu)
-values (
-	0,
-	'0204');
-</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" ht="78.75" x14ac:dyDescent="0.25">
-      <c r="A17" s="6" t="s">
-        <v>182</v>
-      </c>
-      <c r="B17" s="6" t="s">
-        <v>205</v>
-      </c>
-      <c r="C17" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">insert into config_perfil (
-	cod_perfil,
-	cod_item_menu)
-values (
-	0,
-	'0205');
-</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" ht="78.75" x14ac:dyDescent="0.25">
-      <c r="A18" s="6" t="s">
-        <v>182</v>
-      </c>
-      <c r="B18" s="6" t="s">
-        <v>146</v>
-      </c>
-      <c r="C18" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">insert into config_perfil (
-	cod_perfil,
-	cod_item_menu)
-values (
-	0,
-	'03');
-</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" ht="78.75" x14ac:dyDescent="0.25">
-      <c r="A19" s="6" t="s">
-        <v>182</v>
-      </c>
-      <c r="B19" s="6" t="s">
-        <v>196</v>
-      </c>
-      <c r="C19" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">insert into config_perfil (
-	cod_perfil,
-	cod_item_menu)
-values (
-	0,
-	'0301');
-</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" ht="78.75" x14ac:dyDescent="0.25">
-      <c r="A20" s="6" t="s">
-        <v>182</v>
-      </c>
-      <c r="B20" s="6" t="s">
-        <v>197</v>
-      </c>
-      <c r="C20" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">insert into config_perfil (
-	cod_perfil,
-	cod_item_menu)
-values (
-	0,
-	'0302');
-</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" ht="78.75" x14ac:dyDescent="0.25">
-      <c r="A21" s="6" t="s">
-        <v>182</v>
-      </c>
-      <c r="B21" s="6" t="s">
-        <v>198</v>
-      </c>
-      <c r="C21" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">insert into config_perfil (
-	cod_perfil,
-	cod_item_menu)
-values (
-	0,
-	'0303');
-</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" ht="78.75" x14ac:dyDescent="0.25">
-      <c r="A22" s="6" t="s">
-        <v>182</v>
-      </c>
-      <c r="B22" s="6" t="s">
-        <v>199</v>
-      </c>
-      <c r="C22" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">insert into config_perfil (
-	cod_perfil,
-	cod_item_menu)
-values (
-	0,
-	'0304');
-</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" ht="78.75" x14ac:dyDescent="0.25">
-      <c r="A23" s="6" t="s">
-        <v>182</v>
-      </c>
-      <c r="B23" s="6" t="s">
-        <v>200</v>
-      </c>
-      <c r="C23" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">insert into config_perfil (
-	cod_perfil,
-	cod_item_menu)
-values (
-	0,
-	'0305');
-</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" ht="78.75" x14ac:dyDescent="0.25">
-      <c r="A24" s="6" t="s">
-        <v>183</v>
-      </c>
-      <c r="B24" s="6" t="s">
-        <v>140</v>
-      </c>
-      <c r="C24" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">insert into config_perfil (
-	cod_perfil,
-	cod_item_menu)
-values (
-	1,
-	'01');
-</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" ht="78.75" x14ac:dyDescent="0.25">
-      <c r="A25" s="6" t="s">
-        <v>183</v>
-      </c>
-      <c r="B25" s="6" t="s">
-        <v>187</v>
-      </c>
-      <c r="C25" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">insert into config_perfil (
-	cod_perfil,
-	cod_item_menu)
-values (
-	1,
-	'0101');
-</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" ht="78.75" x14ac:dyDescent="0.25">
-      <c r="A26" s="6" t="s">
-        <v>183</v>
-      </c>
-      <c r="B26" s="6" t="s">
-        <v>188</v>
-      </c>
-      <c r="C26" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">insert into config_perfil (
-	cod_perfil,
-	cod_item_menu)
-values (
-	1,
-	'0102');
-</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" ht="78.75" x14ac:dyDescent="0.25">
-      <c r="A27" s="6" t="s">
-        <v>183</v>
-      </c>
-      <c r="B27" s="6" t="s">
-        <v>189</v>
-      </c>
-      <c r="C27" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">insert into config_perfil (
-	cod_perfil,
-	cod_item_menu)
-values (
-	1,
-	'0103');
-</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" ht="78.75" x14ac:dyDescent="0.25">
-      <c r="A28" s="6" t="s">
-        <v>183</v>
-      </c>
-      <c r="B28" s="6" t="s">
-        <v>192</v>
-      </c>
-      <c r="C28" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">insert into config_perfil (
-	cod_perfil,
-	cod_item_menu)
-values (
-	1,
-	'0104');
-</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" ht="78.75" x14ac:dyDescent="0.25">
-      <c r="A29" s="6" t="s">
-        <v>183</v>
-      </c>
-      <c r="B29" s="6" t="s">
-        <v>193</v>
-      </c>
-      <c r="C29" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">insert into config_perfil (
-	cod_perfil,
-	cod_item_menu)
-values (
-	1,
-	'0105');
-</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" ht="78.75" x14ac:dyDescent="0.25">
-      <c r="A30" s="6" t="s">
-        <v>183</v>
-      </c>
-      <c r="B30" s="6" t="s">
-        <v>194</v>
-      </c>
-      <c r="C30" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">insert into config_perfil (
-	cod_perfil,
-	cod_item_menu)
-values (
-	1,
-	'0106');
-</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" ht="78.75" x14ac:dyDescent="0.25">
-      <c r="A31" s="6" t="s">
-        <v>183</v>
-      </c>
-      <c r="B31" s="6" t="s">
-        <v>144</v>
-      </c>
-      <c r="C31" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">insert into config_perfil (
-	cod_perfil,
-	cod_item_menu)
-values (
-	1,
-	'02');
-</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" ht="78.75" x14ac:dyDescent="0.25">
-      <c r="A32" s="6" t="s">
-        <v>183</v>
-      </c>
-      <c r="B32" s="6" t="s">
-        <v>201</v>
-      </c>
-      <c r="C32" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">insert into config_perfil (
-	cod_perfil,
-	cod_item_menu)
-values (
-	1,
-	'0201');
-</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" ht="78.75" x14ac:dyDescent="0.25">
-      <c r="A33" s="6" t="s">
-        <v>183</v>
-      </c>
-      <c r="B33" s="6" t="s">
-        <v>202</v>
-      </c>
-      <c r="C33" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">insert into config_perfil (
-	cod_perfil,
-	cod_item_menu)
-values (
-	1,
-	'0202');
-</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" ht="78.75" x14ac:dyDescent="0.25">
-      <c r="A34" s="6" t="s">
-        <v>183</v>
-      </c>
-      <c r="B34" s="6" t="s">
-        <v>203</v>
-      </c>
-      <c r="C34" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">insert into config_perfil (
-	cod_perfil,
-	cod_item_menu)
-values (
-	1,
-	'0203');
-</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" ht="78.75" x14ac:dyDescent="0.25">
-      <c r="A35" s="6" t="s">
-        <v>183</v>
-      </c>
-      <c r="B35" s="6" t="s">
-        <v>204</v>
-      </c>
-      <c r="C35" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">insert into config_perfil (
-	cod_perfil,
-	cod_item_menu)
-values (
-	1,
-	'0204');
-</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" ht="78.75" x14ac:dyDescent="0.25">
-      <c r="A36" s="6" t="s">
-        <v>183</v>
-      </c>
-      <c r="B36" s="6" t="s">
-        <v>205</v>
-      </c>
-      <c r="C36" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">insert into config_perfil (
-	cod_perfil,
-	cod_item_menu)
-values (
-	1,
-	'0205');
-</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" ht="78.75" x14ac:dyDescent="0.25">
-      <c r="A37" s="6" t="s">
-        <v>183</v>
-      </c>
-      <c r="B37" s="6" t="s">
-        <v>146</v>
-      </c>
-      <c r="C37" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">insert into config_perfil (
-	cod_perfil,
-	cod_item_menu)
-values (
-	1,
-	'03');
-</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" ht="78.75" x14ac:dyDescent="0.25">
-      <c r="A38" s="6" t="s">
-        <v>183</v>
-      </c>
-      <c r="B38" s="6" t="s">
-        <v>196</v>
-      </c>
-      <c r="C38" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">insert into config_perfil (
-	cod_perfil,
-	cod_item_menu)
-values (
-	1,
-	'0301');
-</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" ht="78.75" x14ac:dyDescent="0.25">
-      <c r="A39" s="6" t="s">
-        <v>183</v>
-      </c>
-      <c r="B39" s="6" t="s">
-        <v>197</v>
-      </c>
-      <c r="C39" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">insert into config_perfil (
-	cod_perfil,
-	cod_item_menu)
-values (
-	1,
-	'0302');
-</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" ht="78.75" x14ac:dyDescent="0.25">
-      <c r="A40" s="6" t="s">
-        <v>183</v>
-      </c>
-      <c r="B40" s="6" t="s">
-        <v>198</v>
-      </c>
-      <c r="C40" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">insert into config_perfil (
-	cod_perfil,
-	cod_item_menu)
-values (
-	1,
-	'0303');
-</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" ht="78.75" x14ac:dyDescent="0.25">
-      <c r="A41" s="6" t="s">
-        <v>183</v>
-      </c>
-      <c r="B41" s="6" t="s">
-        <v>199</v>
-      </c>
-      <c r="C41" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">insert into config_perfil (
-	cod_perfil,
-	cod_item_menu)
-values (
-	1,
-	'0304');
-</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" ht="78.75" x14ac:dyDescent="0.25">
-      <c r="A42" s="6" t="s">
-        <v>183</v>
-      </c>
-      <c r="B42" s="6" t="s">
-        <v>200</v>
-      </c>
-      <c r="C42" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">insert into config_perfil (
-	cod_perfil,
-	cod_item_menu)
-values (
-	1,
-	'0305');
-</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" ht="78.75" x14ac:dyDescent="0.25">
-      <c r="A43" s="6" t="s">
-        <v>184</v>
-      </c>
-      <c r="B43" s="6" t="s">
-        <v>140</v>
-      </c>
-      <c r="C43" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">insert into config_perfil (
-	cod_perfil,
-	cod_item_menu)
+        <v xml:space="preserve">insert into agrupador (
+	cod_agrupador,
+	nom_agrupador)
 values (
 	2,
-	'01');
-</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3" ht="78.75" x14ac:dyDescent="0.25">
-      <c r="A44" s="6" t="s">
-        <v>184</v>
-      </c>
-      <c r="B44" s="6" t="s">
-        <v>206</v>
-      </c>
-      <c r="C44" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">insert into config_perfil (
-	cod_perfil,
-	cod_item_menu)
-values (
-	2,
-	'0108');
-</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3" ht="78.75" x14ac:dyDescent="0.25">
-      <c r="A45" s="6" t="s">
-        <v>184</v>
-      </c>
-      <c r="B45" s="6" t="s">
-        <v>144</v>
-      </c>
-      <c r="C45" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">insert into config_perfil (
-	cod_perfil,
-	cod_item_menu)
-values (
-	2,
-	'02');
-</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3" ht="78.75" x14ac:dyDescent="0.25">
-      <c r="A46" s="6" t="s">
-        <v>184</v>
-      </c>
-      <c r="B46" s="6" t="s">
-        <v>201</v>
-      </c>
-      <c r="C46" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">insert into config_perfil (
-	cod_perfil,
-	cod_item_menu)
-values (
-	2,
-	'0201');
+	'Almuerzo personal de servicio');
 </v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{184DDF2A-1EF7-4716-8FBE-A79DA735D726}">
-  <dimension ref="A1:D17"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="18.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="58.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="72.5703125" style="2" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" ht="101.25" x14ac:dyDescent="0.25">
-      <c r="A3" s="1">
-        <v>0</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="C3" s="1">
-        <v>0</v>
-      </c>
-      <c r="D3" s="2" t="str">
-        <f>"insert into "&amp;B$1&amp;" ("&amp;CHAR(10)&amp;
-CHAR(9)&amp;$A$2&amp;","&amp;CHAR(10)&amp;
-CHAR(9)&amp;$B$2&amp;","&amp;CHAR(10)&amp;
-CHAR(9)&amp;$C$2&amp;")"&amp;CHAR(10)&amp;
-"values ("&amp;CHAR(10)&amp;
-CHAR(9)&amp;A3&amp;","&amp;CHAR(10)&amp;
-CHAR(9)&amp;"'"&amp;B3&amp;"',"&amp;CHAR(10)&amp;
-CHAR(9)&amp;C3&amp;");"&amp;CHAR(10)</f>
-        <v xml:space="preserve">insert into agrupador (
-	cod_agrupador,
-	nom_agrupador,
-	cod_tipo_agrupador)
-values (
-	0,
-	'(Sin agrupación)',
-	0);
-</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" ht="101.25" x14ac:dyDescent="0.25">
-      <c r="A4" s="1">
-        <v>1</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C4" s="1">
-        <v>1</v>
-      </c>
-      <c r="D4" s="2" t="str">
-        <f>"insert into "&amp;B$1&amp;" ("&amp;CHAR(10)&amp;
-CHAR(9)&amp;$A$2&amp;","&amp;CHAR(10)&amp;
-CHAR(9)&amp;$B$2&amp;","&amp;CHAR(10)&amp;
-CHAR(9)&amp;$C$2&amp;")"&amp;CHAR(10)&amp;
-"values ("&amp;CHAR(10)&amp;
-CHAR(9)&amp;A4&amp;","&amp;CHAR(10)&amp;
-CHAR(9)&amp;"'"&amp;B4&amp;"',"&amp;CHAR(10)&amp;
-CHAR(9)&amp;C4&amp;");"&amp;CHAR(10)</f>
-        <v xml:space="preserve">insert into agrupador (
-	cod_agrupador,
-	nom_agrupador,
-	cod_tipo_agrupador)
-values (
-	1,
-	'Menú: charquicán y huevo frito, ensalada y postre',
-	1);
-</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" ht="101.25" x14ac:dyDescent="0.25">
-      <c r="A5" s="1">
-        <v>2</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C5" s="1">
-        <v>1</v>
-      </c>
-      <c r="D5" s="2" t="str">
-        <f t="shared" ref="D5:D17" si="0">"insert into "&amp;B$1&amp;" ("&amp;CHAR(10)&amp;
-CHAR(9)&amp;$A$2&amp;","&amp;CHAR(10)&amp;
-CHAR(9)&amp;$B$2&amp;","&amp;CHAR(10)&amp;
-CHAR(9)&amp;$C$2&amp;")"&amp;CHAR(10)&amp;
-"values ("&amp;CHAR(10)&amp;
-CHAR(9)&amp;A5&amp;","&amp;CHAR(10)&amp;
-CHAR(9)&amp;"'"&amp;B5&amp;"',"&amp;CHAR(10)&amp;
-CHAR(9)&amp;C5&amp;");"&amp;CHAR(10)</f>
-        <v xml:space="preserve">insert into agrupador (
-	cod_agrupador,
-	nom_agrupador,
-	cod_tipo_agrupador)
-values (
-	2,
-	'Menú: garbanzos con longaniza, ensalada y postre',
-	1);
-</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="101.25" x14ac:dyDescent="0.25">
-      <c r="A6" s="1">
-        <v>3</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C6" s="1">
-        <v>1</v>
-      </c>
-      <c r="D6" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">insert into agrupador (
-	cod_agrupador,
-	nom_agrupador,
-	cod_tipo_agrupador)
-values (
-	3,
-	'Menú: lentejas con gorda, ensalada y postre',
-	1);
-</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" ht="101.25" x14ac:dyDescent="0.25">
-      <c r="A7" s="1">
-        <v>4</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C7" s="1">
-        <v>1</v>
-      </c>
-      <c r="D7" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">insert into agrupador (
-	cod_agrupador,
-	nom_agrupador,
-	cod_tipo_agrupador)
-values (
-	4,
-	'Menú: pescado horno, puré, ensalada y postre',
-	1);
-</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" ht="101.25" x14ac:dyDescent="0.25">
-      <c r="A8" s="1">
-        <v>5</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C8" s="1">
-        <v>1</v>
-      </c>
-      <c r="D8" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">insert into agrupador (
-	cod_agrupador,
-	nom_agrupador,
-	cod_tipo_agrupador)
-values (
-	5,
-	'Menú: pizza y postre',
-	1);
-</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" ht="101.25" x14ac:dyDescent="0.25">
-      <c r="A9" s="1">
-        <v>6</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="C9" s="1">
-        <v>1</v>
-      </c>
-      <c r="D9" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">insert into agrupador (
-	cod_agrupador,
-	nom_agrupador,
-	cod_tipo_agrupador)
-values (
-	6,
-	'Menú: pollo arvejado y papas doradas, ensalada y postre',
-	1);
-</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" ht="101.25" x14ac:dyDescent="0.25">
-      <c r="A10" s="1">
-        <v>7</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C10" s="1">
-        <v>1</v>
-      </c>
-      <c r="D10" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">insert into agrupador (
-	cod_agrupador,
-	nom_agrupador,
-	cod_tipo_agrupador)
-values (
-	7,
-	'Menú: pollo asado con puré de papas, ensalada y postre',
-	1);
-</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" ht="101.25" x14ac:dyDescent="0.25">
-      <c r="A11" s="1">
-        <v>8</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C11" s="1">
-        <v>1</v>
-      </c>
-      <c r="D11" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">insert into agrupador (
-	cod_agrupador,
-	nom_agrupador,
-	cod_tipo_agrupador)
-values (
-	8,
-	'Menú: Pastel de papa y postre',
-	1);
-</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" ht="101.25" x14ac:dyDescent="0.25">
-      <c r="A12" s="1">
-        <v>9</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="C12" s="1">
-        <v>1</v>
-      </c>
-      <c r="D12" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">insert into agrupador (
-	cod_agrupador,
-	nom_agrupador,
-	cod_tipo_agrupador)
-values (
-	9,
-	'Menú: Arroz chaufa de pollo y postre',
-	1);
-</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" ht="101.25" x14ac:dyDescent="0.25">
-      <c r="A13" s="1">
-        <v>10</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C13" s="1">
-        <v>1</v>
-      </c>
-      <c r="D13" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">insert into agrupador (
-	cod_agrupador,
-	nom_agrupador,
-	cod_tipo_agrupador)
-values (
-	10,
-	'Menú: Garbanzos con longaniza y postre',
-	1);
-</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" ht="101.25" x14ac:dyDescent="0.25">
-      <c r="A14" s="1">
-        <v>11</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C14" s="1">
-        <v>1</v>
-      </c>
-      <c r="D14" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">insert into agrupador (
-	cod_agrupador,
-	nom_agrupador,
-	cod_tipo_agrupador)
-values (
-	11,
-	'Menú: Pasta con salsa de champiñón, aceitunas, perejil y postre',
-	1);
-</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" ht="101.25" x14ac:dyDescent="0.25">
-      <c r="A15" s="1">
-        <v>12</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C15" s="1">
-        <v>1</v>
-      </c>
-      <c r="D15" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">insert into agrupador (
-	cod_agrupador,
-	nom_agrupador,
-	cod_tipo_agrupador)
-values (
-	12,
-	'Menú: Pescado al horno y puré de papas y postre',
-	1);
-</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" ht="101.25" x14ac:dyDescent="0.25">
-      <c r="A16" s="1">
-        <v>13</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C16" s="1">
-        <v>1</v>
-      </c>
-      <c r="D16" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">insert into agrupador (
-	cod_agrupador,
-	nom_agrupador,
-	cod_tipo_agrupador)
-values (
-	13,
-	'Menú: Vacuno Bourguignon, papas asadas y postre',
-	1);
-</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" ht="101.25" x14ac:dyDescent="0.25">
-      <c r="A17" s="1">
-        <v>14</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C17" s="1">
-        <v>1</v>
-      </c>
-      <c r="D17" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">insert into agrupador (
-	cod_agrupador,
-	nom_agrupador,
-	cod_tipo_agrupador)
-values (
-	14,
-	'Menú: Zapallo italiano relleno o guiso, arroz y postre',
-	1);
-</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F8A8934B-F996-4672-8712-8399B293C7D4}">
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="20.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="30.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="27.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="72.5703125" style="2" customWidth="1"/>
-    <col min="5" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" width="20.1796875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="27.26953125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="72.54296875" style="2" customWidth="1"/>
+    <col min="5" max="16384" width="9.1796875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
-        <v>124</v>
+        <v>106</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>125</v>
+        <v>107</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>126</v>
+        <v>108</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" ht="101.25" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="94.5" x14ac:dyDescent="0.35">
       <c r="A3" s="1">
         <v>1</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>127</v>
+        <v>109</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>128</v>
+        <v>110</v>
       </c>
       <c r="D3" s="2" t="str">
         <f>"insert into "&amp;$B$1&amp;" ("&amp;CHAR(10)&amp;
@@ -2413,15 +1105,15 @@
 </v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="101.25" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" ht="94.5" x14ac:dyDescent="0.35">
       <c r="A4" s="1">
         <v>2</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>129</v>
+        <v>111</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>130</v>
+        <v>112</v>
       </c>
       <c r="D4" s="2" t="str">
         <f t="shared" ref="D4:D5" si="0">"insert into "&amp;$B$1&amp;" ("&amp;CHAR(10)&amp;
@@ -2443,15 +1135,15 @@
 </v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="101.25" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" ht="94.5" x14ac:dyDescent="0.35">
       <c r="A5" s="1">
         <v>3</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>131</v>
+        <v>113</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>132</v>
+        <v>114</v>
       </c>
       <c r="D5" s="2" t="str">
         <f t="shared" si="0"/>
@@ -2472,7 +1164,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D3ABF983-4D53-4CD5-B8A8-7865A802CB53}">
   <dimension ref="A1:D4"/>
   <sheetViews>
@@ -2480,45 +1172,45 @@
       <selection activeCell="D3" sqref="D3:D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="18.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="58.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="72.5703125" style="2" customWidth="1"/>
+    <col min="1" max="1" width="18.81640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="58.26953125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="72.54296875" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
-        <v>23</v>
+        <v>6</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>24</v>
+        <v>7</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>25</v>
+        <v>8</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" ht="101.25" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="94.5" x14ac:dyDescent="0.35">
       <c r="A3" s="1">
         <v>1</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>26</v>
+        <v>9</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>42</v>
+        <v>24</v>
       </c>
       <c r="D3" s="2" t="str">
         <f>"insert into "&amp;B$1&amp;" ("&amp;CHAR(10)&amp;
@@ -2540,15 +1232,15 @@
 </v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="101.25" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" ht="94.5" x14ac:dyDescent="0.35">
       <c r="A4" s="1">
         <v>2</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>27</v>
+        <v>10</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>43</v>
+        <v>25</v>
       </c>
       <c r="D4" s="2" t="str">
         <f>"insert into "&amp;B$1&amp;" ("&amp;CHAR(10)&amp;
@@ -2575,44 +1267,44 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{078F4608-0DFF-4D30-B813-CF0C5678B6C3}">
   <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView topLeftCell="A10" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="18.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="58.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="72.5703125" style="2" customWidth="1"/>
+    <col min="1" max="1" width="18.81640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="58.26953125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="72.54296875" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
-        <v>28</v>
+        <v>11</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>29</v>
+        <v>12</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" ht="90" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="73.5" x14ac:dyDescent="0.35">
       <c r="A3" s="1">
         <v>1</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>36</v>
+        <v>19</v>
       </c>
       <c r="C3" s="2" t="str">
         <f>"insert into "&amp;B$1&amp;" ("&amp;CHAR(10)&amp;
@@ -2630,12 +1322,12 @@
 </v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="78.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" ht="73.5" x14ac:dyDescent="0.35">
       <c r="A4" s="1">
         <v>2</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>33</v>
+        <v>16</v>
       </c>
       <c r="C4" s="2" t="str">
         <f t="shared" ref="C4:C12" si="0">"insert into "&amp;B$1&amp;" ("&amp;CHAR(10)&amp;
@@ -2653,12 +1345,12 @@
 </v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="78.75" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" ht="73.5" x14ac:dyDescent="0.35">
       <c r="A5" s="1">
         <v>3</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>37</v>
+        <v>20</v>
       </c>
       <c r="C5" s="2" t="str">
         <f t="shared" si="0"/>
@@ -2671,12 +1363,12 @@
 </v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="78.75" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" ht="73.5" x14ac:dyDescent="0.35">
       <c r="A6" s="1">
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>34</v>
+        <v>17</v>
       </c>
       <c r="C6" s="2" t="str">
         <f t="shared" si="0"/>
@@ -2689,12 +1381,12 @@
 </v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="78.75" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" ht="73.5" x14ac:dyDescent="0.35">
       <c r="A7" s="1">
         <v>5</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>39</v>
+        <v>22</v>
       </c>
       <c r="C7" s="2" t="str">
         <f t="shared" si="0"/>
@@ -2707,12 +1399,12 @@
 </v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="78.75" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" ht="73.5" x14ac:dyDescent="0.35">
       <c r="A8" s="1">
         <v>6</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>31</v>
+        <v>14</v>
       </c>
       <c r="C8" s="2" t="str">
         <f t="shared" si="0"/>
@@ -2725,12 +1417,12 @@
 </v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="78.75" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" ht="73.5" x14ac:dyDescent="0.35">
       <c r="A9" s="1">
         <v>7</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>40</v>
+        <v>23</v>
       </c>
       <c r="C9" s="2" t="str">
         <f t="shared" si="0"/>
@@ -2743,12 +1435,12 @@
 </v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="78.75" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" ht="73.5" x14ac:dyDescent="0.35">
       <c r="A10" s="1">
         <v>8</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>38</v>
+        <v>21</v>
       </c>
       <c r="C10" s="2" t="str">
         <f t="shared" si="0"/>
@@ -2761,12 +1453,12 @@
 </v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="78.75" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" ht="73.5" x14ac:dyDescent="0.35">
       <c r="A11" s="1">
         <v>9</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>32</v>
+        <v>15</v>
       </c>
       <c r="C11" s="2" t="str">
         <f t="shared" si="0"/>
@@ -2779,12 +1471,12 @@
 </v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="78.75" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" ht="73.5" x14ac:dyDescent="0.35">
       <c r="A12" s="1">
         <v>10</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>35</v>
+        <v>18</v>
       </c>
       <c r="C12" s="2" t="str">
         <f t="shared" si="0"/>
@@ -2805,7 +1497,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2DE28EA-1421-45F3-9D3B-EBBDF2870481}">
   <dimension ref="A1:F8"/>
   <sheetViews>
@@ -2813,59 +1505,59 @@
       <selection activeCell="F3" sqref="F3:F8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="18.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="58.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="26.140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="26.140625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="24.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="72.5703125" style="2" customWidth="1"/>
+    <col min="1" max="1" width="18.81640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="58.26953125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26.1796875" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="26.1796875" style="1" customWidth="1"/>
+    <col min="5" max="5" width="24.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="72.54296875" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
-        <v>45</v>
+        <v>27</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>46</v>
+        <v>28</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>47</v>
+        <v>29</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>48</v>
+        <v>30</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>49</v>
+        <v>31</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" ht="146.25" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="136.5" x14ac:dyDescent="0.35">
       <c r="A3" s="1">
         <v>1</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>57</v>
+        <v>39</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>51</v>
+        <v>33</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>60</v>
+        <v>42</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>60</v>
+        <v>42</v>
       </c>
       <c r="F3" s="2" t="str">
         <f t="shared" ref="F3:F8" si="0">"insert into "&amp;B$1&amp;" ("&amp;CHAR(10)&amp;
@@ -2895,15 +1587,15 @@
 </v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="146.25" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" ht="136.5" x14ac:dyDescent="0.35">
       <c r="A4" s="1">
         <v>2</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>54</v>
+        <v>36</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>50</v>
+        <v>32</v>
       </c>
       <c r="D4" s="1">
         <v>2</v>
@@ -2928,21 +1620,21 @@
 </v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="146.25" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" ht="136.5" x14ac:dyDescent="0.35">
       <c r="A5" s="1">
         <v>3</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>55</v>
+        <v>37</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>52</v>
+        <v>34</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>60</v>
+        <v>42</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>60</v>
+        <v>42</v>
       </c>
       <c r="F5" s="2" t="str">
         <f t="shared" si="0"/>
@@ -2961,15 +1653,15 @@
 </v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="146.25" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" ht="136.5" x14ac:dyDescent="0.35">
       <c r="A6" s="1">
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>61</v>
+        <v>43</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>62</v>
+        <v>44</v>
       </c>
       <c r="D6" s="1">
         <v>3</v>
@@ -2994,21 +1686,21 @@
 </v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="146.25" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" ht="136.5" x14ac:dyDescent="0.35">
       <c r="A7" s="1">
         <v>5</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>58</v>
+        <v>40</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>59</v>
+        <v>41</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>60</v>
+        <v>42</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>60</v>
+        <v>42</v>
       </c>
       <c r="F7" s="2" t="str">
         <f t="shared" si="0"/>
@@ -3027,21 +1719,21 @@
 </v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="146.25" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" ht="136.5" x14ac:dyDescent="0.35">
       <c r="A8" s="1">
         <v>6</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>56</v>
+        <v>38</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>53</v>
+        <v>35</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>60</v>
+        <v>42</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>60</v>
+        <v>42</v>
       </c>
       <c r="F8" s="2" t="str">
         <f t="shared" si="0"/>
@@ -3068,7 +1760,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5869A447-B67B-431A-B703-A4F7C1093F1B}">
   <dimension ref="A1:E18"/>
   <sheetViews>
@@ -3076,50 +1768,50 @@
       <selection sqref="A1:E1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="18.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="58.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="26.140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="26.140625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="72.5703125" style="2" customWidth="1"/>
-    <col min="6" max="16384" width="11.42578125" style="1"/>
+    <col min="1" max="1" width="18.81640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="58.26953125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26.1796875" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="26.1796875" style="1" customWidth="1"/>
+    <col min="5" max="5" width="72.54296875" style="2" customWidth="1"/>
+    <col min="6" max="16384" width="11.453125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
-        <v>63</v>
+        <v>45</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>64</v>
+        <v>46</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>65</v>
+        <v>47</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>23</v>
+        <v>6</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" ht="123.75" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="115.5" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
-        <v>67</v>
+        <v>49</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>68</v>
+        <v>50</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>99</v>
+        <v>81</v>
       </c>
       <c r="D3" s="1">
         <v>2</v>
@@ -3148,15 +1840,15 @@
 </v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="123.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="115.5" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
-        <v>69</v>
+        <v>51</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>70</v>
+        <v>52</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>100</v>
+        <v>82</v>
       </c>
       <c r="D4" s="1">
         <v>2</v>
@@ -3185,15 +1877,15 @@
 </v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="123.75" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" ht="115.5" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
-        <v>71</v>
+        <v>53</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>72</v>
+        <v>54</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>102</v>
+        <v>84</v>
       </c>
       <c r="D5" s="1">
         <v>2</v>
@@ -3213,15 +1905,15 @@
 </v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="123.75" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" ht="115.5" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
-        <v>73</v>
+        <v>55</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>74</v>
+        <v>56</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>101</v>
+        <v>83</v>
       </c>
       <c r="D6" s="1">
         <v>2</v>
@@ -3241,15 +1933,15 @@
 </v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="123.75" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" ht="115.5" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
-        <v>75</v>
+        <v>57</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>76</v>
+        <v>58</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>103</v>
+        <v>85</v>
       </c>
       <c r="D7" s="1">
         <v>2</v>
@@ -3269,15 +1961,15 @@
 </v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="123.75" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" ht="115.5" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
-        <v>77</v>
+        <v>59</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>78</v>
+        <v>60</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>104</v>
+        <v>86</v>
       </c>
       <c r="D8" s="1">
         <v>1</v>
@@ -3297,15 +1989,15 @@
 </v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="123.75" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" ht="115.5" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
-        <v>79</v>
+        <v>61</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>80</v>
+        <v>62</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>100</v>
+        <v>82</v>
       </c>
       <c r="D9" s="1">
         <v>1</v>
@@ -3325,15 +2017,15 @@
 </v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="123.75" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" ht="115.5" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
-        <v>81</v>
+        <v>63</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>82</v>
+        <v>64</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>106</v>
+        <v>88</v>
       </c>
       <c r="D10" s="1">
         <v>1</v>
@@ -3353,15 +2045,15 @@
 </v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="123.75" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" ht="115.5" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
-        <v>83</v>
+        <v>65</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>84</v>
+        <v>66</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>111</v>
+        <v>93</v>
       </c>
       <c r="D11" s="1">
         <v>1</v>
@@ -3381,15 +2073,15 @@
 </v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="123.75" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" ht="115.5" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
-        <v>85</v>
+        <v>67</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>86</v>
+        <v>68</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>107</v>
+        <v>89</v>
       </c>
       <c r="D12" s="1">
         <v>1</v>
@@ -3409,15 +2101,15 @@
 </v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="123.75" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" ht="115.5" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
-        <v>87</v>
+        <v>69</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>88</v>
+        <v>70</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>108</v>
+        <v>90</v>
       </c>
       <c r="D13" s="1">
         <v>1</v>
@@ -3437,15 +2129,15 @@
 </v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="123.75" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" ht="115.5" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
-        <v>89</v>
+        <v>71</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>90</v>
+        <v>72</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>109</v>
+        <v>91</v>
       </c>
       <c r="D14" s="1">
         <v>1</v>
@@ -3465,15 +2157,15 @@
 </v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="123.75" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" ht="115.5" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
-        <v>91</v>
+        <v>73</v>
       </c>
       <c r="B15" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="C15" s="3" t="s">
         <v>92</v>
-      </c>
-      <c r="C15" s="3" t="s">
-        <v>110</v>
       </c>
       <c r="D15" s="1">
         <v>1</v>
@@ -3493,15 +2185,15 @@
 </v>
       </c>
     </row>
-    <row r="16" spans="1:5" ht="123.75" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" ht="115.5" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
-        <v>93</v>
+        <v>75</v>
       </c>
       <c r="B16" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="C16" s="3" t="s">
         <v>94</v>
-      </c>
-      <c r="C16" s="3" t="s">
-        <v>112</v>
       </c>
       <c r="D16" s="1">
         <v>1</v>
@@ -3521,15 +2213,15 @@
 </v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="123.75" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" ht="115.5" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="C17" s="3" t="s">
         <v>95</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="C17" s="3" t="s">
-        <v>113</v>
       </c>
       <c r="D17" s="1">
         <v>1</v>
@@ -3549,15 +2241,15 @@
 </v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="123.75" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" ht="115.5" x14ac:dyDescent="0.35">
       <c r="A18" s="1" t="s">
-        <v>97</v>
+        <v>79</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>98</v>
+        <v>80</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>105</v>
+        <v>87</v>
       </c>
       <c r="D18" s="1">
         <v>1</v>
@@ -3582,7 +2274,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8559A7F4-4B2D-41BA-8E2B-AD35723212BD}">
   <dimension ref="A1:D5"/>
   <sheetViews>
@@ -3590,45 +2282,45 @@
       <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="18.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="58.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="26.140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="72.5703125" style="2" customWidth="1"/>
+    <col min="1" max="1" width="18.81640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="58.26953125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26.1796875" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="72.54296875" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
-        <v>114</v>
+        <v>96</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>116</v>
+        <v>98</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>117</v>
+        <v>99</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" ht="101.25" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="94.5" x14ac:dyDescent="0.35">
       <c r="A3" s="1">
         <v>0</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>118</v>
+        <v>100</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>120</v>
+        <v>102</v>
       </c>
       <c r="D3" s="2" t="str">
         <f>"insert into "&amp;B$1&amp;" ("&amp;CHAR(10)&amp;
@@ -3650,15 +2342,15 @@
 </v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="101.25" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" ht="94.5" x14ac:dyDescent="0.35">
       <c r="A4" s="1">
         <v>1</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>135</v>
+        <v>115</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>121</v>
+        <v>103</v>
       </c>
       <c r="D4" s="2" t="str">
         <f t="shared" ref="D4:D5" si="0">"insert into "&amp;B$1&amp;" ("&amp;CHAR(10)&amp;
@@ -3680,15 +2372,15 @@
 </v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="101.25" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" ht="94.5" x14ac:dyDescent="0.35">
       <c r="A5" s="1">
         <v>2</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>119</v>
+        <v>101</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>122</v>
+        <v>104</v>
       </c>
       <c r="D5" s="2" t="str">
         <f t="shared" si="0"/>
@@ -3708,7 +2400,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4C63790F-D7B5-42A7-B7A6-A107E7362141}">
   <dimension ref="A1:F24"/>
   <sheetViews>
@@ -3716,58 +2408,58 @@
       <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="18.85546875" style="6" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="26.85546875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="51.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="41.28515625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="41.28515625" style="6" customWidth="1"/>
-    <col min="6" max="6" width="72.5703125" style="1" customWidth="1"/>
-    <col min="7" max="16384" width="11.42578125" style="1"/>
+    <col min="1" max="1" width="18.81640625" style="6" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.81640625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="51.1796875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="41.26953125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="41.26953125" style="6" customWidth="1"/>
+    <col min="6" max="6" width="72.54296875" style="1" customWidth="1"/>
+    <col min="7" max="16384" width="11.453125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" s="5" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>137</v>
+        <v>117</v>
       </c>
       <c r="F1" s="2"/>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" s="5" t="s">
-        <v>136</v>
+        <v>116</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>138</v>
+        <v>118</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>117</v>
+        <v>99</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>142</v>
+        <v>122</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>139</v>
+        <v>119</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" ht="146.25" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="136.5" x14ac:dyDescent="0.35">
       <c r="A3" s="6" t="s">
-        <v>140</v>
+        <v>120</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>185</v>
+        <v>165</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>186</v>
+        <v>166</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>60</v>
+        <v>42</v>
       </c>
       <c r="F3" s="2" t="str">
         <f>"insert into "&amp;B$1&amp;" ("&amp;CHAR(10)&amp;
@@ -3797,21 +2489,21 @@
 </v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="146.25" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" ht="136.5" x14ac:dyDescent="0.35">
       <c r="A4" s="6" t="s">
-        <v>187</v>
+        <v>167</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>141</v>
+        <v>121</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>162</v>
+        <v>142</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>143</v>
+        <v>123</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>140</v>
+        <v>120</v>
       </c>
       <c r="F4" s="2" t="str">
         <f t="shared" ref="F4:F23" si="0">"insert into "&amp;B$1&amp;" ("&amp;CHAR(10)&amp;
@@ -3841,18 +2533,18 @@
 </v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="146.25" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" ht="136.5" x14ac:dyDescent="0.35">
       <c r="A5" s="6" t="s">
-        <v>188</v>
+        <v>168</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>190</v>
+        <v>170</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>191</v>
+        <v>171</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>140</v>
+        <v>120</v>
       </c>
       <c r="F5" s="2" t="str">
         <f t="shared" si="0"/>
@@ -3871,21 +2563,21 @@
 </v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="146.25" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" ht="136.5" x14ac:dyDescent="0.35">
       <c r="A6" s="6" t="s">
-        <v>189</v>
+        <v>169</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>145</v>
+        <v>125</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>163</v>
+        <v>143</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>168</v>
+        <v>148</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>140</v>
+        <v>120</v>
       </c>
       <c r="F6" s="2" t="str">
         <f t="shared" si="0"/>
@@ -3904,21 +2596,21 @@
 </v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="146.25" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" ht="136.5" x14ac:dyDescent="0.35">
       <c r="A7" s="6" t="s">
-        <v>192</v>
+        <v>172</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>147</v>
+        <v>127</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>164</v>
+        <v>144</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>169</v>
+        <v>149</v>
       </c>
       <c r="E7" s="6" t="s">
-        <v>140</v>
+        <v>120</v>
       </c>
       <c r="F7" s="2" t="str">
         <f t="shared" si="0"/>
@@ -3937,18 +2629,18 @@
 </v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="146.25" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" ht="136.5" x14ac:dyDescent="0.35">
       <c r="A8" s="6" t="s">
-        <v>193</v>
+        <v>173</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>190</v>
+        <v>170</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>191</v>
+        <v>171</v>
       </c>
       <c r="E8" s="6" t="s">
-        <v>140</v>
+        <v>120</v>
       </c>
       <c r="F8" s="2" t="str">
         <f t="shared" si="0"/>
@@ -3967,21 +2659,21 @@
 </v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="146.25" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" ht="136.5" x14ac:dyDescent="0.35">
       <c r="A9" s="6" t="s">
-        <v>194</v>
+        <v>174</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>150</v>
+        <v>130</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>164</v>
+        <v>144</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>207</v>
+        <v>187</v>
       </c>
       <c r="E9" s="6" t="s">
-        <v>140</v>
+        <v>120</v>
       </c>
       <c r="F9" s="2" t="str">
         <f t="shared" si="0"/>
@@ -4000,18 +2692,18 @@
 </v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="146.25" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" ht="136.5" x14ac:dyDescent="0.35">
       <c r="A10" s="6" t="s">
-        <v>195</v>
+        <v>175</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>190</v>
+        <v>170</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>191</v>
+        <v>171</v>
       </c>
       <c r="E10" s="6" t="s">
-        <v>140</v>
+        <v>120</v>
       </c>
       <c r="F10" s="2" t="str">
         <f t="shared" si="0"/>
@@ -4030,21 +2722,21 @@
 </v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="146.25" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" ht="136.5" x14ac:dyDescent="0.35">
       <c r="A11" s="6" t="s">
-        <v>206</v>
+        <v>186</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>151</v>
+        <v>131</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>167</v>
+        <v>147</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>170</v>
+        <v>150</v>
       </c>
       <c r="E11" s="6" t="s">
-        <v>140</v>
+        <v>120</v>
       </c>
       <c r="F11" s="2" t="str">
         <f t="shared" si="0"/>
@@ -4063,21 +2755,21 @@
 </v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="146.25" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" ht="136.5" x14ac:dyDescent="0.35">
       <c r="A12" s="6" t="s">
-        <v>144</v>
+        <v>124</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>149</v>
+        <v>129</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>166</v>
+        <v>146</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>60</v>
+        <v>42</v>
       </c>
       <c r="E12" s="6" t="s">
-        <v>60</v>
+        <v>42</v>
       </c>
       <c r="F12" s="2" t="str">
         <f t="shared" si="0"/>
@@ -4096,21 +2788,21 @@
 </v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="168" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" ht="168" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="6" t="s">
-        <v>201</v>
+        <v>181</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>157</v>
+        <v>137</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>157</v>
+        <v>137</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>172</v>
+        <v>152</v>
       </c>
       <c r="E13" s="6" t="s">
-        <v>144</v>
+        <v>124</v>
       </c>
       <c r="F13" s="2" t="str">
         <f t="shared" si="0"/>
@@ -4129,21 +2821,21 @@
 </v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="146.25" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" ht="136.5" x14ac:dyDescent="0.35">
       <c r="A14" s="6" t="s">
-        <v>202</v>
+        <v>182</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>158</v>
+        <v>138</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>158</v>
+        <v>138</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>174</v>
+        <v>154</v>
       </c>
       <c r="E14" s="6" t="s">
-        <v>144</v>
+        <v>124</v>
       </c>
       <c r="F14" s="2" t="str">
         <f t="shared" si="0"/>
@@ -4162,21 +2854,21 @@
 </v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="146.25" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" ht="136.5" x14ac:dyDescent="0.35">
       <c r="A15" s="6" t="s">
-        <v>203</v>
+        <v>183</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>159</v>
+        <v>139</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>159</v>
+        <v>139</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>175</v>
+        <v>155</v>
       </c>
       <c r="E15" s="6" t="s">
-        <v>144</v>
+        <v>124</v>
       </c>
       <c r="F15" s="2" t="str">
         <f t="shared" si="0"/>
@@ -4195,21 +2887,21 @@
 </v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="146.25" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" ht="136.5" x14ac:dyDescent="0.35">
       <c r="A16" s="6" t="s">
-        <v>204</v>
+        <v>184</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>160</v>
+        <v>140</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>160</v>
+        <v>140</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>176</v>
+        <v>156</v>
       </c>
       <c r="E16" s="6" t="s">
-        <v>144</v>
+        <v>124</v>
       </c>
       <c r="F16" s="2" t="str">
         <f t="shared" si="0"/>
@@ -4228,21 +2920,21 @@
 </v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="146.25" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" ht="136.5" x14ac:dyDescent="0.35">
       <c r="A17" s="6" t="s">
-        <v>205</v>
+        <v>185</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>161</v>
+        <v>141</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>161</v>
+        <v>141</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>177</v>
+        <v>157</v>
       </c>
       <c r="E17" s="6" t="s">
-        <v>144</v>
+        <v>124</v>
       </c>
       <c r="F17" s="2" t="str">
         <f t="shared" si="0"/>
@@ -4261,21 +2953,21 @@
 </v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="146.25" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" ht="136.5" x14ac:dyDescent="0.35">
       <c r="A18" s="6" t="s">
-        <v>146</v>
+        <v>126</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>148</v>
+        <v>128</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>165</v>
+        <v>145</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>60</v>
+        <v>42</v>
       </c>
       <c r="E18" s="6" t="s">
-        <v>60</v>
+        <v>42</v>
       </c>
       <c r="F18" s="2" t="str">
         <f t="shared" si="0"/>
@@ -4294,21 +2986,21 @@
 </v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="146.25" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" ht="136.5" x14ac:dyDescent="0.35">
       <c r="A19" s="6" t="s">
-        <v>196</v>
+        <v>176</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>152</v>
+        <v>132</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>152</v>
+        <v>132</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>171</v>
+        <v>151</v>
       </c>
       <c r="E19" s="6" t="s">
-        <v>146</v>
+        <v>126</v>
       </c>
       <c r="F19" s="2" t="str">
         <f t="shared" si="0"/>
@@ -4327,21 +3019,21 @@
 </v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="146.25" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" ht="136.5" x14ac:dyDescent="0.35">
       <c r="A20" s="6" t="s">
-        <v>197</v>
+        <v>177</v>
       </c>
       <c r="B20" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="D20" s="1" t="s">
         <v>153</v>
       </c>
-      <c r="C20" s="1" t="s">
-        <v>153</v>
-      </c>
-      <c r="D20" s="1" t="s">
-        <v>173</v>
-      </c>
       <c r="E20" s="6" t="s">
-        <v>146</v>
+        <v>126</v>
       </c>
       <c r="F20" s="2" t="str">
         <f t="shared" si="0"/>
@@ -4360,21 +3052,21 @@
 </v>
       </c>
     </row>
-    <row r="21" spans="1:6" ht="146.25" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" ht="136.5" x14ac:dyDescent="0.35">
       <c r="A21" s="6" t="s">
-        <v>198</v>
+        <v>178</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>154</v>
+        <v>134</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>154</v>
+        <v>134</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>178</v>
+        <v>158</v>
       </c>
       <c r="E21" s="6" t="s">
-        <v>146</v>
+        <v>126</v>
       </c>
       <c r="F21" s="2" t="str">
         <f t="shared" si="0"/>
@@ -4393,21 +3085,21 @@
 </v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="146.25" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" ht="136.5" x14ac:dyDescent="0.35">
       <c r="A22" s="6" t="s">
-        <v>199</v>
+        <v>179</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>155</v>
+        <v>135</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>155</v>
+        <v>135</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>179</v>
+        <v>159</v>
       </c>
       <c r="E22" s="6" t="s">
-        <v>146</v>
+        <v>126</v>
       </c>
       <c r="F22" s="2" t="str">
         <f t="shared" si="0"/>
@@ -4426,21 +3118,21 @@
 </v>
       </c>
     </row>
-    <row r="23" spans="1:6" ht="146.25" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" ht="136.5" x14ac:dyDescent="0.35">
       <c r="A23" s="6" t="s">
-        <v>200</v>
+        <v>180</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>156</v>
+        <v>136</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>156</v>
+        <v>136</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>180</v>
+        <v>160</v>
       </c>
       <c r="E23" s="6" t="s">
-        <v>146</v>
+        <v>126</v>
       </c>
       <c r="F23" s="2" t="str">
         <f t="shared" si="0"/>
@@ -4459,7 +3151,7 @@
 </v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
       <c r="F24" s="2"/>
     </row>
   </sheetData>
@@ -4469,4 +3161,847 @@
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7280E62-DF8A-463C-91EE-0993A8577DEA}">
+  <dimension ref="A1:C46"/>
+  <sheetViews>
+    <sheetView topLeftCell="A41" workbookViewId="0">
+      <selection activeCell="C43" sqref="C43"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="18.81640625" style="6" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.81640625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="72.54296875" style="1" customWidth="1"/>
+    <col min="4" max="16384" width="11.453125" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="C1" s="2"/>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A2" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="78.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="6" t="s">
+        <v>162</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>120</v>
+      </c>
+      <c r="C3" s="2" t="str">
+        <f>"insert into "&amp;B$1&amp;" ("&amp;CHAR(10)&amp;
+CHAR(9)&amp;$A$2&amp;","&amp;CHAR(10)&amp;
+CHAR(9)&amp;$B$2&amp;")"&amp;CHAR(10)&amp;
+"values ("&amp;CHAR(10)&amp;
+CHAR(9)&amp;A3&amp;","&amp;CHAR(10)&amp;
+CHAR(9)&amp;"'"&amp;B3&amp;"');"&amp;CHAR(10)</f>
+        <v xml:space="preserve">insert into config_perfil (
+	cod_perfil,
+	cod_item_menu)
+values (
+	0,
+	'01');
+</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="73.5" x14ac:dyDescent="0.35">
+      <c r="A4" s="6" t="s">
+        <v>162</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>167</v>
+      </c>
+      <c r="C4" s="2" t="str">
+        <f t="shared" ref="C4:C46" si="0">"insert into "&amp;B$1&amp;" ("&amp;CHAR(10)&amp;
+CHAR(9)&amp;$A$2&amp;","&amp;CHAR(10)&amp;
+CHAR(9)&amp;$B$2&amp;")"&amp;CHAR(10)&amp;
+"values ("&amp;CHAR(10)&amp;
+CHAR(9)&amp;A4&amp;","&amp;CHAR(10)&amp;
+CHAR(9)&amp;"'"&amp;B4&amp;"');"&amp;CHAR(10)</f>
+        <v xml:space="preserve">insert into config_perfil (
+	cod_perfil,
+	cod_item_menu)
+values (
+	0,
+	'0101');
+</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="73.5" x14ac:dyDescent="0.35">
+      <c r="A5" s="6" t="s">
+        <v>162</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>168</v>
+      </c>
+      <c r="C5" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">insert into config_perfil (
+	cod_perfil,
+	cod_item_menu)
+values (
+	0,
+	'0102');
+</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="73.5" x14ac:dyDescent="0.35">
+      <c r="A6" s="6" t="s">
+        <v>162</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>169</v>
+      </c>
+      <c r="C6" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">insert into config_perfil (
+	cod_perfil,
+	cod_item_menu)
+values (
+	0,
+	'0103');
+</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="73.5" x14ac:dyDescent="0.35">
+      <c r="A7" s="6" t="s">
+        <v>162</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>172</v>
+      </c>
+      <c r="C7" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">insert into config_perfil (
+	cod_perfil,
+	cod_item_menu)
+values (
+	0,
+	'0104');
+</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="73.5" x14ac:dyDescent="0.35">
+      <c r="A8" s="6" t="s">
+        <v>162</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>173</v>
+      </c>
+      <c r="C8" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">insert into config_perfil (
+	cod_perfil,
+	cod_item_menu)
+values (
+	0,
+	'0105');
+</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="73.5" x14ac:dyDescent="0.35">
+      <c r="A9" s="6" t="s">
+        <v>162</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>174</v>
+      </c>
+      <c r="C9" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">insert into config_perfil (
+	cod_perfil,
+	cod_item_menu)
+values (
+	0,
+	'0106');
+</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="73.5" x14ac:dyDescent="0.35">
+      <c r="A10" s="6" t="s">
+        <v>162</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>175</v>
+      </c>
+      <c r="C10" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">insert into config_perfil (
+	cod_perfil,
+	cod_item_menu)
+values (
+	0,
+	'0107');
+</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="73.5" x14ac:dyDescent="0.35">
+      <c r="A11" s="6" t="s">
+        <v>162</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>186</v>
+      </c>
+      <c r="C11" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">insert into config_perfil (
+	cod_perfil,
+	cod_item_menu)
+values (
+	0,
+	'0108');
+</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="73.5" x14ac:dyDescent="0.35">
+      <c r="A12" s="6" t="s">
+        <v>162</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>124</v>
+      </c>
+      <c r="C12" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">insert into config_perfil (
+	cod_perfil,
+	cod_item_menu)
+values (
+	0,
+	'02');
+</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="73.5" x14ac:dyDescent="0.35">
+      <c r="A13" s="6" t="s">
+        <v>162</v>
+      </c>
+      <c r="B13" s="6" t="s">
+        <v>181</v>
+      </c>
+      <c r="C13" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">insert into config_perfil (
+	cod_perfil,
+	cod_item_menu)
+values (
+	0,
+	'0201');
+</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="73.5" x14ac:dyDescent="0.35">
+      <c r="A14" s="6" t="s">
+        <v>162</v>
+      </c>
+      <c r="B14" s="6" t="s">
+        <v>182</v>
+      </c>
+      <c r="C14" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">insert into config_perfil (
+	cod_perfil,
+	cod_item_menu)
+values (
+	0,
+	'0202');
+</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="73.5" x14ac:dyDescent="0.35">
+      <c r="A15" s="6" t="s">
+        <v>162</v>
+      </c>
+      <c r="B15" s="6" t="s">
+        <v>183</v>
+      </c>
+      <c r="C15" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">insert into config_perfil (
+	cod_perfil,
+	cod_item_menu)
+values (
+	0,
+	'0203');
+</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="73.5" x14ac:dyDescent="0.35">
+      <c r="A16" s="6" t="s">
+        <v>162</v>
+      </c>
+      <c r="B16" s="6" t="s">
+        <v>184</v>
+      </c>
+      <c r="C16" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">insert into config_perfil (
+	cod_perfil,
+	cod_item_menu)
+values (
+	0,
+	'0204');
+</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="73.5" x14ac:dyDescent="0.35">
+      <c r="A17" s="6" t="s">
+        <v>162</v>
+      </c>
+      <c r="B17" s="6" t="s">
+        <v>185</v>
+      </c>
+      <c r="C17" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">insert into config_perfil (
+	cod_perfil,
+	cod_item_menu)
+values (
+	0,
+	'0205');
+</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="73.5" x14ac:dyDescent="0.35">
+      <c r="A18" s="6" t="s">
+        <v>162</v>
+      </c>
+      <c r="B18" s="6" t="s">
+        <v>126</v>
+      </c>
+      <c r="C18" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">insert into config_perfil (
+	cod_perfil,
+	cod_item_menu)
+values (
+	0,
+	'03');
+</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="73.5" x14ac:dyDescent="0.35">
+      <c r="A19" s="6" t="s">
+        <v>162</v>
+      </c>
+      <c r="B19" s="6" t="s">
+        <v>176</v>
+      </c>
+      <c r="C19" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">insert into config_perfil (
+	cod_perfil,
+	cod_item_menu)
+values (
+	0,
+	'0301');
+</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="73.5" x14ac:dyDescent="0.35">
+      <c r="A20" s="6" t="s">
+        <v>162</v>
+      </c>
+      <c r="B20" s="6" t="s">
+        <v>177</v>
+      </c>
+      <c r="C20" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">insert into config_perfil (
+	cod_perfil,
+	cod_item_menu)
+values (
+	0,
+	'0302');
+</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="73.5" x14ac:dyDescent="0.35">
+      <c r="A21" s="6" t="s">
+        <v>162</v>
+      </c>
+      <c r="B21" s="6" t="s">
+        <v>178</v>
+      </c>
+      <c r="C21" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">insert into config_perfil (
+	cod_perfil,
+	cod_item_menu)
+values (
+	0,
+	'0303');
+</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" ht="73.5" x14ac:dyDescent="0.35">
+      <c r="A22" s="6" t="s">
+        <v>162</v>
+      </c>
+      <c r="B22" s="6" t="s">
+        <v>179</v>
+      </c>
+      <c r="C22" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">insert into config_perfil (
+	cod_perfil,
+	cod_item_menu)
+values (
+	0,
+	'0304');
+</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" ht="73.5" x14ac:dyDescent="0.35">
+      <c r="A23" s="6" t="s">
+        <v>162</v>
+      </c>
+      <c r="B23" s="6" t="s">
+        <v>180</v>
+      </c>
+      <c r="C23" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">insert into config_perfil (
+	cod_perfil,
+	cod_item_menu)
+values (
+	0,
+	'0305');
+</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" ht="73.5" x14ac:dyDescent="0.35">
+      <c r="A24" s="6" t="s">
+        <v>163</v>
+      </c>
+      <c r="B24" s="6" t="s">
+        <v>120</v>
+      </c>
+      <c r="C24" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">insert into config_perfil (
+	cod_perfil,
+	cod_item_menu)
+values (
+	1,
+	'01');
+</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" ht="73.5" x14ac:dyDescent="0.35">
+      <c r="A25" s="6" t="s">
+        <v>163</v>
+      </c>
+      <c r="B25" s="6" t="s">
+        <v>167</v>
+      </c>
+      <c r="C25" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">insert into config_perfil (
+	cod_perfil,
+	cod_item_menu)
+values (
+	1,
+	'0101');
+</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" ht="73.5" x14ac:dyDescent="0.35">
+      <c r="A26" s="6" t="s">
+        <v>163</v>
+      </c>
+      <c r="B26" s="6" t="s">
+        <v>168</v>
+      </c>
+      <c r="C26" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">insert into config_perfil (
+	cod_perfil,
+	cod_item_menu)
+values (
+	1,
+	'0102');
+</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" ht="73.5" x14ac:dyDescent="0.35">
+      <c r="A27" s="6" t="s">
+        <v>163</v>
+      </c>
+      <c r="B27" s="6" t="s">
+        <v>169</v>
+      </c>
+      <c r="C27" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">insert into config_perfil (
+	cod_perfil,
+	cod_item_menu)
+values (
+	1,
+	'0103');
+</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" ht="73.5" x14ac:dyDescent="0.35">
+      <c r="A28" s="6" t="s">
+        <v>163</v>
+      </c>
+      <c r="B28" s="6" t="s">
+        <v>172</v>
+      </c>
+      <c r="C28" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">insert into config_perfil (
+	cod_perfil,
+	cod_item_menu)
+values (
+	1,
+	'0104');
+</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" ht="73.5" x14ac:dyDescent="0.35">
+      <c r="A29" s="6" t="s">
+        <v>163</v>
+      </c>
+      <c r="B29" s="6" t="s">
+        <v>173</v>
+      </c>
+      <c r="C29" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">insert into config_perfil (
+	cod_perfil,
+	cod_item_menu)
+values (
+	1,
+	'0105');
+</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" ht="73.5" x14ac:dyDescent="0.35">
+      <c r="A30" s="6" t="s">
+        <v>163</v>
+      </c>
+      <c r="B30" s="6" t="s">
+        <v>174</v>
+      </c>
+      <c r="C30" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">insert into config_perfil (
+	cod_perfil,
+	cod_item_menu)
+values (
+	1,
+	'0106');
+</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" ht="73.5" x14ac:dyDescent="0.35">
+      <c r="A31" s="6" t="s">
+        <v>163</v>
+      </c>
+      <c r="B31" s="6" t="s">
+        <v>124</v>
+      </c>
+      <c r="C31" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">insert into config_perfil (
+	cod_perfil,
+	cod_item_menu)
+values (
+	1,
+	'02');
+</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" ht="73.5" x14ac:dyDescent="0.35">
+      <c r="A32" s="6" t="s">
+        <v>163</v>
+      </c>
+      <c r="B32" s="6" t="s">
+        <v>181</v>
+      </c>
+      <c r="C32" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">insert into config_perfil (
+	cod_perfil,
+	cod_item_menu)
+values (
+	1,
+	'0201');
+</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" ht="73.5" x14ac:dyDescent="0.35">
+      <c r="A33" s="6" t="s">
+        <v>163</v>
+      </c>
+      <c r="B33" s="6" t="s">
+        <v>182</v>
+      </c>
+      <c r="C33" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">insert into config_perfil (
+	cod_perfil,
+	cod_item_menu)
+values (
+	1,
+	'0202');
+</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" ht="73.5" x14ac:dyDescent="0.35">
+      <c r="A34" s="6" t="s">
+        <v>163</v>
+      </c>
+      <c r="B34" s="6" t="s">
+        <v>183</v>
+      </c>
+      <c r="C34" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">insert into config_perfil (
+	cod_perfil,
+	cod_item_menu)
+values (
+	1,
+	'0203');
+</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" ht="73.5" x14ac:dyDescent="0.35">
+      <c r="A35" s="6" t="s">
+        <v>163</v>
+      </c>
+      <c r="B35" s="6" t="s">
+        <v>184</v>
+      </c>
+      <c r="C35" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">insert into config_perfil (
+	cod_perfil,
+	cod_item_menu)
+values (
+	1,
+	'0204');
+</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" ht="73.5" x14ac:dyDescent="0.35">
+      <c r="A36" s="6" t="s">
+        <v>163</v>
+      </c>
+      <c r="B36" s="6" t="s">
+        <v>185</v>
+      </c>
+      <c r="C36" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">insert into config_perfil (
+	cod_perfil,
+	cod_item_menu)
+values (
+	1,
+	'0205');
+</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" ht="73.5" x14ac:dyDescent="0.35">
+      <c r="A37" s="6" t="s">
+        <v>163</v>
+      </c>
+      <c r="B37" s="6" t="s">
+        <v>126</v>
+      </c>
+      <c r="C37" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">insert into config_perfil (
+	cod_perfil,
+	cod_item_menu)
+values (
+	1,
+	'03');
+</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" ht="73.5" x14ac:dyDescent="0.35">
+      <c r="A38" s="6" t="s">
+        <v>163</v>
+      </c>
+      <c r="B38" s="6" t="s">
+        <v>176</v>
+      </c>
+      <c r="C38" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">insert into config_perfil (
+	cod_perfil,
+	cod_item_menu)
+values (
+	1,
+	'0301');
+</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" ht="73.5" x14ac:dyDescent="0.35">
+      <c r="A39" s="6" t="s">
+        <v>163</v>
+      </c>
+      <c r="B39" s="6" t="s">
+        <v>177</v>
+      </c>
+      <c r="C39" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">insert into config_perfil (
+	cod_perfil,
+	cod_item_menu)
+values (
+	1,
+	'0302');
+</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" ht="73.5" x14ac:dyDescent="0.35">
+      <c r="A40" s="6" t="s">
+        <v>163</v>
+      </c>
+      <c r="B40" s="6" t="s">
+        <v>178</v>
+      </c>
+      <c r="C40" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">insert into config_perfil (
+	cod_perfil,
+	cod_item_menu)
+values (
+	1,
+	'0303');
+</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" ht="73.5" x14ac:dyDescent="0.35">
+      <c r="A41" s="6" t="s">
+        <v>163</v>
+      </c>
+      <c r="B41" s="6" t="s">
+        <v>179</v>
+      </c>
+      <c r="C41" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">insert into config_perfil (
+	cod_perfil,
+	cod_item_menu)
+values (
+	1,
+	'0304');
+</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" ht="73.5" x14ac:dyDescent="0.35">
+      <c r="A42" s="6" t="s">
+        <v>163</v>
+      </c>
+      <c r="B42" s="6" t="s">
+        <v>180</v>
+      </c>
+      <c r="C42" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">insert into config_perfil (
+	cod_perfil,
+	cod_item_menu)
+values (
+	1,
+	'0305');
+</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" ht="73.5" x14ac:dyDescent="0.35">
+      <c r="A43" s="6" t="s">
+        <v>164</v>
+      </c>
+      <c r="B43" s="6" t="s">
+        <v>120</v>
+      </c>
+      <c r="C43" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">insert into config_perfil (
+	cod_perfil,
+	cod_item_menu)
+values (
+	2,
+	'01');
+</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" ht="73.5" x14ac:dyDescent="0.35">
+      <c r="A44" s="6" t="s">
+        <v>164</v>
+      </c>
+      <c r="B44" s="6" t="s">
+        <v>186</v>
+      </c>
+      <c r="C44" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">insert into config_perfil (
+	cod_perfil,
+	cod_item_menu)
+values (
+	2,
+	'0108');
+</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" ht="73.5" x14ac:dyDescent="0.35">
+      <c r="A45" s="6" t="s">
+        <v>164</v>
+      </c>
+      <c r="B45" s="6" t="s">
+        <v>124</v>
+      </c>
+      <c r="C45" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">insert into config_perfil (
+	cod_perfil,
+	cod_item_menu)
+values (
+	2,
+	'02');
+</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" ht="73.5" x14ac:dyDescent="0.35">
+      <c r="A46" s="6" t="s">
+        <v>164</v>
+      </c>
+      <c r="B46" s="6" t="s">
+        <v>181</v>
+      </c>
+      <c r="C46" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">insert into config_perfil (
+	cod_perfil,
+	cod_item_menu)
+values (
+	2,
+	'0201');
+</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>